<commit_message>
order created date in excel sheet, final change d2d-v1
</commit_message>
<xml_diff>
--- a/webroot/invoice/order_5_invoice.xlsx
+++ b/webroot/invoice/order_5_invoice.xlsx
@@ -41,7 +41,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2016-01-12</t>
+    <t>2017-01-08</t>
   </si>
   <si>
     <t>Contact</t>
@@ -50,7 +50,7 @@
     <t>Time</t>
   </si>
   <si>
-    <t>12:25</t>
+    <t>00:56:00</t>
   </si>
   <si>
     <t>My ID</t>

</xml_diff>